<commit_message>
Am completat exelul cu power consumption
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Botix\Desktop\TDC\TDC\src\PELib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex5\OneDrive\Desktop\Git\TDC\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C6689-1657-4B11-ABCC-CD7D65FAE658}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="318">
   <si>
     <t>74AC00</t>
   </si>
@@ -1069,16 +1070,91 @@
     <t>74AC244 Buffer Tri-State</t>
   </si>
   <si>
-    <t>4 pf</t>
-  </si>
-  <si>
-    <t>https://www.futurlec.com/74AC/74AC244.shtml</t>
+    <t>https://www.futurlec.com/74AC/74AC244.shtmll</t>
+  </si>
+  <si>
+    <t>4.5pF</t>
+  </si>
+  <si>
+    <t>4 pF</t>
+  </si>
+  <si>
+    <t>74ACT244</t>
+  </si>
+  <si>
+    <t>Buffer Tri-State</t>
+  </si>
+  <si>
+    <t>80uA</t>
+  </si>
+  <si>
+    <t>8uA</t>
+  </si>
+  <si>
+    <t>http://pdf1.alldatasheet.com/datasheet-pdf/view/21758/STMICROELECTRONICS/74ACT244.html</t>
+  </si>
+  <si>
+    <t>5pF</t>
+  </si>
+  <si>
+    <t>4pF</t>
+  </si>
+  <si>
+    <t>3.8pF</t>
+  </si>
+  <si>
+    <t>3.5pF</t>
+  </si>
+  <si>
+    <t>74HC244</t>
+  </si>
+  <si>
+    <t>34pF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ds/2/308/74HC244-D-310411.pdf</t>
+  </si>
+  <si>
+    <t>https://assets.nexperia.com/documents/data-sheet/74HC_HCT244.pdf</t>
+  </si>
+  <si>
+    <t>160uA</t>
+  </si>
+  <si>
+    <t>74LS126</t>
+  </si>
+  <si>
+    <t>12mA</t>
+  </si>
+  <si>
+    <t>22mA</t>
+  </si>
+  <si>
+    <t>https://www.futurlec.com/74LS/74LS126.shtml</t>
+  </si>
+  <si>
+    <t>74F125</t>
+  </si>
+  <si>
+    <t>https://www.futurlec.com/74F/74F125.shtml</t>
+  </si>
+  <si>
+    <t>31.7mA</t>
+  </si>
+  <si>
+    <t>18.5mA</t>
+  </si>
+  <si>
+    <t>6pF</t>
+  </si>
+  <si>
+    <t>7.5pF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1449,11 +1525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,6 +1581,9 @@
       <c r="E2" t="s">
         <v>64</v>
       </c>
+      <c r="F2" t="s">
+        <v>292</v>
+      </c>
       <c r="G2" t="s">
         <v>62</v>
       </c>
@@ -1528,6 +1607,9 @@
       <c r="E3" t="s">
         <v>64</v>
       </c>
+      <c r="F3" t="s">
+        <v>292</v>
+      </c>
       <c r="G3" t="s">
         <v>62</v>
       </c>
@@ -1577,6 +1659,9 @@
       <c r="E5" t="s">
         <v>64</v>
       </c>
+      <c r="F5" t="s">
+        <v>292</v>
+      </c>
       <c r="G5" t="s">
         <v>69</v>
       </c>
@@ -1600,6 +1685,9 @@
       <c r="E6" t="s">
         <v>64</v>
       </c>
+      <c r="F6" t="s">
+        <v>292</v>
+      </c>
       <c r="G6" t="s">
         <v>70</v>
       </c>
@@ -1623,6 +1711,9 @@
       <c r="E7" t="s">
         <v>64</v>
       </c>
+      <c r="F7" t="s">
+        <v>292</v>
+      </c>
       <c r="G7" t="s">
         <v>71</v>
       </c>
@@ -1646,6 +1737,9 @@
       <c r="E8" t="s">
         <v>64</v>
       </c>
+      <c r="F8" t="s">
+        <v>292</v>
+      </c>
       <c r="G8" t="s">
         <v>69</v>
       </c>
@@ -1669,6 +1763,9 @@
       <c r="E9" t="s">
         <v>64</v>
       </c>
+      <c r="F9" t="s">
+        <v>292</v>
+      </c>
       <c r="G9" t="s">
         <v>72</v>
       </c>
@@ -1690,38 +1787,39 @@
         <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G10" t="s">
         <v>110</v>
       </c>
-      <c r="H10" t="s">
-        <v>292</v>
+      <c r="H10" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
-    <hyperlink ref="H5" r:id="rId5"/>
-    <hyperlink ref="H6" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{FEEFF108-170F-4BCC-B622-0501F5B75D38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,11 +1827,11 @@
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1747,13 +1845,16 @@
         <v>138</v>
       </c>
       <c r="F1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1770,13 +1871,16 @@
         <v>144</v>
       </c>
       <c r="F2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1792,11 +1896,14 @@
       <c r="E3" t="s">
         <v>142</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1813,13 +1920,16 @@
         <v>144</v>
       </c>
       <c r="F4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1835,11 +1945,14 @@
       <c r="E5" t="s">
         <v>142</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1856,13 +1969,16 @@
         <v>144</v>
       </c>
       <c r="F6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1878,11 +1994,14 @@
       <c r="E7" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1898,11 +2017,14 @@
       <c r="E8" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1918,11 +2040,14 @@
       <c r="E9" t="s">
         <v>144</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1939,13 +2064,16 @@
         <v>144</v>
       </c>
       <c r="F10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G10" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1962,13 +2090,16 @@
         <v>144</v>
       </c>
       <c r="F11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G11" t="s">
         <v>156</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1981,11 +2112,14 @@
       <c r="D12" t="s">
         <v>158</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12" t="s">
+        <v>317</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -2001,11 +2135,14 @@
       <c r="E13" t="s">
         <v>144</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" t="s">
+        <v>299</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -2021,11 +2158,14 @@
       <c r="E14" t="s">
         <v>144</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2042,13 +2182,16 @@
         <v>144</v>
       </c>
       <c r="F15" t="s">
+        <v>299</v>
+      </c>
+      <c r="G15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2064,11 +2207,14 @@
       <c r="E16" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="F16" t="s">
+        <v>299</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2085,13 +2231,16 @@
         <v>144</v>
       </c>
       <c r="F17" t="s">
+        <v>299</v>
+      </c>
+      <c r="G17" t="s">
         <v>156</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2107,11 +2256,14 @@
       <c r="E18" t="s">
         <v>144</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="F18" t="s">
+        <v>299</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2127,49 +2279,52 @@
       <c r="E19" t="s">
         <v>168</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>299</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml"/>
-    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml"/>
-    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml"/>
-    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml"/>
-    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml"/>
-    <hyperlink ref="G2" r:id="rId9"/>
-    <hyperlink ref="G3" r:id="rId10"/>
-    <hyperlink ref="G4" r:id="rId11"/>
-    <hyperlink ref="G5" r:id="rId12"/>
-    <hyperlink ref="G6" r:id="rId13"/>
-    <hyperlink ref="G7" r:id="rId14"/>
-    <hyperlink ref="G8" r:id="rId15"/>
-    <hyperlink ref="G9" r:id="rId16"/>
-    <hyperlink ref="G10" r:id="rId17"/>
-    <hyperlink ref="G11" r:id="rId18"/>
-    <hyperlink ref="G12" r:id="rId19"/>
-    <hyperlink ref="G13" r:id="rId20"/>
-    <hyperlink ref="G14" r:id="rId21"/>
-    <hyperlink ref="G15" r:id="rId22"/>
-    <hyperlink ref="G16" r:id="rId23"/>
-    <hyperlink ref="G17" r:id="rId24"/>
-    <hyperlink ref="G18" r:id="rId25"/>
-    <hyperlink ref="G19" r:id="rId26"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="H4" r:id="rId11" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
+    <hyperlink ref="H5" r:id="rId12" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
+    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0900-00000C000000}"/>
+    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0900-00000D000000}"/>
+    <hyperlink ref="H8" r:id="rId15" xr:uid="{00000000-0004-0000-0900-00000E000000}"/>
+    <hyperlink ref="H9" r:id="rId16" xr:uid="{00000000-0004-0000-0900-00000F000000}"/>
+    <hyperlink ref="H10" r:id="rId17" xr:uid="{00000000-0004-0000-0900-000010000000}"/>
+    <hyperlink ref="H11" r:id="rId18" xr:uid="{00000000-0004-0000-0900-000011000000}"/>
+    <hyperlink ref="H12" r:id="rId19" xr:uid="{00000000-0004-0000-0900-000012000000}"/>
+    <hyperlink ref="H13" r:id="rId20" xr:uid="{00000000-0004-0000-0900-000013000000}"/>
+    <hyperlink ref="H14" r:id="rId21" xr:uid="{00000000-0004-0000-0900-000014000000}"/>
+    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0900-000015000000}"/>
+    <hyperlink ref="H16" r:id="rId23" xr:uid="{00000000-0004-0000-0900-000016000000}"/>
+    <hyperlink ref="H17" r:id="rId24" xr:uid="{00000000-0004-0000-0900-000017000000}"/>
+    <hyperlink ref="H18" r:id="rId25" xr:uid="{00000000-0004-0000-0900-000018000000}"/>
+    <hyperlink ref="H19" r:id="rId26" xr:uid="{00000000-0004-0000-0900-000019000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,6 +2376,9 @@
       <c r="E2" t="s">
         <v>64</v>
       </c>
+      <c r="F2" t="s">
+        <v>292</v>
+      </c>
       <c r="G2" t="s">
         <v>62</v>
       </c>
@@ -2244,6 +2402,9 @@
       <c r="E3" t="s">
         <v>78</v>
       </c>
+      <c r="F3" t="s">
+        <v>292</v>
+      </c>
       <c r="G3" t="s">
         <v>62</v>
       </c>
@@ -2267,6 +2428,9 @@
       <c r="E4" t="s">
         <v>78</v>
       </c>
+      <c r="F4" t="s">
+        <v>292</v>
+      </c>
       <c r="G4" t="s">
         <v>62</v>
       </c>
@@ -2290,6 +2454,9 @@
       <c r="E5" t="s">
         <v>78</v>
       </c>
+      <c r="F5" t="s">
+        <v>292</v>
+      </c>
       <c r="G5" t="s">
         <v>69</v>
       </c>
@@ -2313,6 +2480,9 @@
       <c r="E6" t="s">
         <v>78</v>
       </c>
+      <c r="F6" t="s">
+        <v>292</v>
+      </c>
       <c r="G6" t="s">
         <v>70</v>
       </c>
@@ -2336,6 +2506,9 @@
       <c r="E7" t="s">
         <v>78</v>
       </c>
+      <c r="F7" t="s">
+        <v>301</v>
+      </c>
       <c r="G7" t="s">
         <v>92</v>
       </c>
@@ -2359,6 +2532,9 @@
       <c r="E8" t="s">
         <v>78</v>
       </c>
+      <c r="F8" t="s">
+        <v>292</v>
+      </c>
       <c r="G8" t="s">
         <v>69</v>
       </c>
@@ -2382,6 +2558,9 @@
       <c r="E9" t="s">
         <v>64</v>
       </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
       <c r="G9" t="s">
         <v>62</v>
       </c>
@@ -2389,41 +2568,69 @@
         <v>93</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>297</v>
+      </c>
+      <c r="E10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" t="s">
+        <v>300</v>
+      </c>
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H8" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{A73F30B2-2E69-47FC-AFC2-6147E741D374}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -2440,13 +2647,16 @@
         <v>126</v>
       </c>
       <c r="G1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2466,13 +2676,16 @@
         <v>78</v>
       </c>
       <c r="G2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2492,13 +2705,16 @@
         <v>78</v>
       </c>
       <c r="G3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H3" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
@@ -2518,13 +2734,16 @@
         <v>78</v>
       </c>
       <c r="G4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -2544,13 +2763,16 @@
         <v>78</v>
       </c>
       <c r="G5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -2570,13 +2792,16 @@
         <v>78</v>
       </c>
       <c r="G6" t="s">
+        <v>302</v>
+      </c>
+      <c r="H6" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -2596,13 +2821,16 @@
         <v>78</v>
       </c>
       <c r="G7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H7" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -2622,13 +2850,16 @@
         <v>78</v>
       </c>
       <c r="G8" t="s">
+        <v>302</v>
+      </c>
+      <c r="H8" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -2648,47 +2879,81 @@
         <v>78</v>
       </c>
       <c r="G9" t="s">
+        <v>302</v>
+      </c>
+      <c r="H9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" t="s">
+        <v>304</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{05F9B0C7-93CD-4C31-A677-8F901FFD7270}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -2705,13 +2970,16 @@
         <v>126</v>
       </c>
       <c r="G1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2731,13 +2999,16 @@
         <v>78</v>
       </c>
       <c r="G2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" t="s">
         <v>99</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -2757,13 +3028,16 @@
         <v>78</v>
       </c>
       <c r="G3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H3" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -2783,13 +3057,16 @@
         <v>78</v>
       </c>
       <c r="G4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H4" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -2809,13 +3086,16 @@
         <v>78</v>
       </c>
       <c r="G5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2835,13 +3115,16 @@
         <v>78</v>
       </c>
       <c r="G6" t="s">
+        <v>302</v>
+      </c>
+      <c r="H6" t="s">
         <v>121</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2861,13 +3144,16 @@
         <v>78</v>
       </c>
       <c r="G7" t="s">
+        <v>302</v>
+      </c>
+      <c r="H7" t="s">
         <v>127</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -2887,13 +3173,16 @@
         <v>78</v>
       </c>
       <c r="G8" t="s">
+        <v>302</v>
+      </c>
+      <c r="H8" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>136</v>
       </c>
@@ -2913,33 +3202,66 @@
         <v>78</v>
       </c>
       <c r="G9" t="s">
+        <v>302</v>
+      </c>
+      <c r="H9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>303</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>297</v>
+      </c>
+      <c r="E10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" t="s">
+        <v>307</v>
+      </c>
+      <c r="G10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H7" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{0A1A1C8D-D838-4302-9C22-7CBF01312669}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3091,25 +3413,28 @@
         <v>230</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,23 +3626,44 @@
         <v>203</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E10" t="s">
+        <v>310</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{CB09BBD4-8CA2-4EAD-B9C3-A2A6F5393421}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3470,22 +3816,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3677,23 +4023,44 @@
         <v>262</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E10" t="s">
+        <v>315</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{2DB22402-2296-4707-AE8C-C220A483C513}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3811,10 +4178,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
update on isetc paper
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex5\OneDrive\Desktop\Git\TDC\src\PELib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Botix\Desktop\TDC\TDC\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7C6689-1657-4B11-ABCC-CD7D65FAE658}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="321">
   <si>
     <t>74AC00</t>
   </si>
@@ -1070,9 +1069,6 @@
     <t>74AC244 Buffer Tri-State</t>
   </si>
   <si>
-    <t>https://www.futurlec.com/74AC/74AC244.shtmll</t>
-  </si>
-  <si>
     <t>4.5pF</t>
   </si>
   <si>
@@ -1149,12 +1145,24 @@
   </si>
   <si>
     <t>7.5pF</t>
+  </si>
+  <si>
+    <t>21pf</t>
+  </si>
+  <si>
+    <t>45pf</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/149/74AC244-888494.pdf</t>
+  </si>
+  <si>
+    <t>https://www.futurlec.com/74AC/74AC244.shtml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1525,11 +1533,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1590,7 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G2" t="s">
         <v>62</v>
@@ -1608,7 +1616,7 @@
         <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -1660,7 +1668,7 @@
         <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G5" t="s">
         <v>69</v>
@@ -1686,7 +1694,7 @@
         <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
@@ -1712,7 +1720,7 @@
         <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G7" t="s">
         <v>71</v>
@@ -1738,7 +1746,7 @@
         <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G8" t="s">
         <v>69</v>
@@ -1764,7 +1772,7 @@
         <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G9" t="s">
         <v>72</v>
@@ -1787,34 +1795,58 @@
         <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>317</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>291</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>290</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F11" t="s">
+        <v>289</v>
+      </c>
+      <c r="G11" t="s">
+        <v>318</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{FEEFF108-170F-4BCC-B622-0501F5B75D38}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H9" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="H6" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -1871,7 +1903,7 @@
         <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G2" t="s">
         <v>121</v>
@@ -1897,7 +1929,7 @@
         <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>143</v>
@@ -1920,7 +1952,7 @@
         <v>144</v>
       </c>
       <c r="F4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G4" t="s">
         <v>121</v>
@@ -1946,7 +1978,7 @@
         <v>142</v>
       </c>
       <c r="F5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>146</v>
@@ -1969,7 +2001,7 @@
         <v>144</v>
       </c>
       <c r="F6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G6" t="s">
         <v>127</v>
@@ -1995,7 +2027,7 @@
         <v>142</v>
       </c>
       <c r="F7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>148</v>
@@ -2018,7 +2050,7 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>151</v>
@@ -2041,7 +2073,7 @@
         <v>144</v>
       </c>
       <c r="F9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>153</v>
@@ -2064,7 +2096,7 @@
         <v>144</v>
       </c>
       <c r="F10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G10" t="s">
         <v>120</v>
@@ -2090,7 +2122,7 @@
         <v>144</v>
       </c>
       <c r="F11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G11" t="s">
         <v>156</v>
@@ -2113,7 +2145,7 @@
         <v>158</v>
       </c>
       <c r="F12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>159</v>
@@ -2136,7 +2168,7 @@
         <v>144</v>
       </c>
       <c r="F13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>160</v>
@@ -2159,7 +2191,7 @@
         <v>144</v>
       </c>
       <c r="F14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>161</v>
@@ -2182,7 +2214,7 @@
         <v>144</v>
       </c>
       <c r="F15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G15" t="s">
         <v>69</v>
@@ -2208,7 +2240,7 @@
         <v>144</v>
       </c>
       <c r="F16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>164</v>
@@ -2231,7 +2263,7 @@
         <v>144</v>
       </c>
       <c r="F17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G17" t="s">
         <v>156</v>
@@ -2257,7 +2289,7 @@
         <v>144</v>
       </c>
       <c r="F18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>166</v>
@@ -2280,7 +2312,7 @@
         <v>168</v>
       </c>
       <c r="F19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>169</v>
@@ -2288,39 +2320,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
-    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
-    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
-    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
-    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
-    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
-    <hyperlink ref="H3" r:id="rId10" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
-    <hyperlink ref="H4" r:id="rId11" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
-    <hyperlink ref="H5" r:id="rId12" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
-    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0900-00000C000000}"/>
-    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0900-00000D000000}"/>
-    <hyperlink ref="H8" r:id="rId15" xr:uid="{00000000-0004-0000-0900-00000E000000}"/>
-    <hyperlink ref="H9" r:id="rId16" xr:uid="{00000000-0004-0000-0900-00000F000000}"/>
-    <hyperlink ref="H10" r:id="rId17" xr:uid="{00000000-0004-0000-0900-000010000000}"/>
-    <hyperlink ref="H11" r:id="rId18" xr:uid="{00000000-0004-0000-0900-000011000000}"/>
-    <hyperlink ref="H12" r:id="rId19" xr:uid="{00000000-0004-0000-0900-000012000000}"/>
-    <hyperlink ref="H13" r:id="rId20" xr:uid="{00000000-0004-0000-0900-000013000000}"/>
-    <hyperlink ref="H14" r:id="rId21" xr:uid="{00000000-0004-0000-0900-000014000000}"/>
-    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0900-000015000000}"/>
-    <hyperlink ref="H16" r:id="rId23" xr:uid="{00000000-0004-0000-0900-000016000000}"/>
-    <hyperlink ref="H17" r:id="rId24" xr:uid="{00000000-0004-0000-0900-000017000000}"/>
-    <hyperlink ref="H18" r:id="rId25" xr:uid="{00000000-0004-0000-0900-000018000000}"/>
-    <hyperlink ref="H19" r:id="rId26" xr:uid="{00000000-0004-0000-0900-000019000000}"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml"/>
+    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml"/>
+    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml"/>
+    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml"/>
+    <hyperlink ref="H2" r:id="rId9"/>
+    <hyperlink ref="H3" r:id="rId10"/>
+    <hyperlink ref="H4" r:id="rId11"/>
+    <hyperlink ref="H5" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="H7" r:id="rId14"/>
+    <hyperlink ref="H8" r:id="rId15"/>
+    <hyperlink ref="H9" r:id="rId16"/>
+    <hyperlink ref="H10" r:id="rId17"/>
+    <hyperlink ref="H11" r:id="rId18"/>
+    <hyperlink ref="H12" r:id="rId19"/>
+    <hyperlink ref="H13" r:id="rId20"/>
+    <hyperlink ref="H14" r:id="rId21"/>
+    <hyperlink ref="H15" r:id="rId22"/>
+    <hyperlink ref="H16" r:id="rId23"/>
+    <hyperlink ref="H17" r:id="rId24"/>
+    <hyperlink ref="H18" r:id="rId25"/>
+    <hyperlink ref="H19" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2377,7 +2409,7 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G2" t="s">
         <v>62</v>
@@ -2403,7 +2435,7 @@
         <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -2429,7 +2461,7 @@
         <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G4" t="s">
         <v>62</v>
@@ -2455,7 +2487,7 @@
         <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G5" t="s">
         <v>69</v>
@@ -2481,7 +2513,7 @@
         <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G6" t="s">
         <v>70</v>
@@ -2507,7 +2539,7 @@
         <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G7" t="s">
         <v>92</v>
@@ -2533,7 +2565,7 @@
         <v>78</v>
       </c>
       <c r="F8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G8" t="s">
         <v>69</v>
@@ -2559,7 +2591,7 @@
         <v>64</v>
       </c>
       <c r="F9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G9" t="s">
         <v>62</v>
@@ -2570,48 +2602,48 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" t="s">
         <v>294</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" t="s">
         <v>295</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>297</v>
-      </c>
-      <c r="E10" t="s">
-        <v>296</v>
-      </c>
       <c r="F10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G10" t="s">
         <v>105</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{A73F30B2-2E69-47FC-AFC2-6147E741D374}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H8" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2676,7 +2708,7 @@
         <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H2" t="s">
         <v>99</v>
@@ -2705,7 +2737,7 @@
         <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H3" t="s">
         <v>99</v>
@@ -2734,7 +2766,7 @@
         <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H4" t="s">
         <v>110</v>
@@ -2763,7 +2795,7 @@
         <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H5" t="s">
         <v>115</v>
@@ -2792,7 +2824,7 @@
         <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H6" t="s">
         <v>120</v>
@@ -2821,7 +2853,7 @@
         <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H7" t="s">
         <v>99</v>
@@ -2850,7 +2882,7 @@
         <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H8" t="s">
         <v>132</v>
@@ -2879,7 +2911,7 @@
         <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H9" t="s">
         <v>62</v>
@@ -2890,10 +2922,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2911,30 +2943,30 @@
         <v>115</v>
       </c>
       <c r="H10" t="s">
+        <v>303</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>305</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{05F9B0C7-93CD-4C31-A677-8F901FFD7270}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2999,7 +3031,7 @@
         <v>78</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H2" t="s">
         <v>99</v>
@@ -3028,7 +3060,7 @@
         <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H3" t="s">
         <v>105</v>
@@ -3057,7 +3089,7 @@
         <v>78</v>
       </c>
       <c r="G4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H4" t="s">
         <v>105</v>
@@ -3086,7 +3118,7 @@
         <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H5" t="s">
         <v>69</v>
@@ -3115,7 +3147,7 @@
         <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H6" t="s">
         <v>121</v>
@@ -3144,7 +3176,7 @@
         <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H7" t="s">
         <v>127</v>
@@ -3173,7 +3205,7 @@
         <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H8" t="s">
         <v>133</v>
@@ -3202,7 +3234,7 @@
         <v>78</v>
       </c>
       <c r="G9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H9" t="s">
         <v>62</v>
@@ -3213,51 +3245,51 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" t="s">
         <v>295</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>297</v>
-      </c>
-      <c r="E10" t="s">
-        <v>296</v>
-      </c>
       <c r="F10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H10" t="s">
         <v>72</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{0A1A1C8D-D838-4302-9C22-7CBF01312669}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3418,19 +3450,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3628,42 +3660,42 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>308</v>
       </c>
-      <c r="B10" t="s">
-        <v>295</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>309</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{CB09BBD4-8CA2-4EAD-B9C3-A2A6F5393421}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3816,18 +3848,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4025,42 +4057,42 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E10" t="s">
+        <v>314</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B10" t="s">
-        <v>295</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>314</v>
-      </c>
-      <c r="E10" t="s">
-        <v>315</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{2DB22402-2296-4707-AE8C-C220A483C513}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4178,10 +4210,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
insert Vcc port  in modules Signed-off-by: Iulia Chereja <chereja_iulia@yahoo.com>
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Botix\Desktop\TDC\TDC\src\PELib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iulia\Desktop\repo\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DD29B7-F19F-4B88-ADA2-DC86FDF36294}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -1162,7 +1163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1533,7 +1534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1829,16 +1830,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
-    <hyperlink ref="H5" r:id="rId5"/>
-    <hyperlink ref="H6" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H8" r:id="rId8"/>
-    <hyperlink ref="H10" r:id="rId9"/>
-    <hyperlink ref="H11" r:id="rId10"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
@@ -1846,10 +1847,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1964,10 +1965,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1975,7 +1976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2251,26 +2252,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H8" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H9" r:id="rId8"/>
-    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,7 +2281,7 @@
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
@@ -2574,25 +2575,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2603,7 +2604,7 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
@@ -2897,22 +2898,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -3386,39 +3387,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml"/>
-    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml"/>
-    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml"/>
-    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml"/>
-    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml"/>
-    <hyperlink ref="H2" r:id="rId9"/>
-    <hyperlink ref="H3" r:id="rId10"/>
-    <hyperlink ref="H4" r:id="rId11"/>
-    <hyperlink ref="H5" r:id="rId12"/>
-    <hyperlink ref="H6" r:id="rId13"/>
-    <hyperlink ref="H7" r:id="rId14"/>
-    <hyperlink ref="H8" r:id="rId15"/>
-    <hyperlink ref="H9" r:id="rId16"/>
-    <hyperlink ref="H10" r:id="rId17"/>
-    <hyperlink ref="H11" r:id="rId18"/>
-    <hyperlink ref="H12" r:id="rId19"/>
-    <hyperlink ref="H13" r:id="rId20"/>
-    <hyperlink ref="H14" r:id="rId21"/>
-    <hyperlink ref="H15" r:id="rId22"/>
-    <hyperlink ref="H16" r:id="rId23"/>
-    <hyperlink ref="H17" r:id="rId24"/>
-    <hyperlink ref="H18" r:id="rId25"/>
-    <hyperlink ref="H19" r:id="rId26"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="H4" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="H5" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="H8" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="H9" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="H10" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="H11" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="H12" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="H13" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="H14" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="H16" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="H17" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="H18" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="H19" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3579,19 +3580,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3809,22 +3810,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3977,18 +3978,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4206,15 +4207,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G8" r:id="rId7"/>
-    <hyperlink ref="G9" r:id="rId8"/>
-    <hyperlink ref="G10" r:id="rId9"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Signed-off-by: Iulia Chereja <chereja_iulia@yahoo.com>
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iulia\Desktop\repo\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DD29B7-F19F-4B88-ADA2-DC86FDF36294}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E345711-3A64-42C4-ABE3-8C480FF62FFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
     <sheet name="74act" sheetId="2" r:id="rId2"/>
     <sheet name="74hc" sheetId="6" r:id="rId3"/>
     <sheet name="74hct" sheetId="7" r:id="rId4"/>
-    <sheet name="4000" sheetId="10" r:id="rId5"/>
+    <sheet name="CMOS" sheetId="10" r:id="rId5"/>
     <sheet name="74als" sheetId="3" r:id="rId6"/>
     <sheet name="74ls" sheetId="4" r:id="rId7"/>
     <sheet name="74lvc" sheetId="5" r:id="rId8"/>
@@ -1850,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2917,8 +2917,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
renamed .ignore.txt files to .gitignore (not te save 0.bak files); other updates
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iulia\Desktop\repo\src\PELib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Botix\Desktop\TDC\TDC\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E345711-3A64-42C4-ABE3-8C480FF62FFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="322">
   <si>
     <t>74AC00</t>
   </si>
@@ -1159,11 +1158,37 @@
   <si>
     <t>https://www.futurlec.com/74AC/74AC244.shtml</t>
   </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (@ TA = +25°C) max</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1534,7 +1559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1830,16 +1855,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H9" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="H6" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H8" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
@@ -1847,7 +1872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1965,10 +1990,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1976,7 +2001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2252,26 +2277,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="H9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H8" r:id="rId6"/>
+    <hyperlink ref="H7" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,7 +2319,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>321</v>
       </c>
       <c r="E1" t="s">
         <v>68</v>
@@ -2381,7 +2406,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
         <v>64</v>
@@ -2410,7 +2435,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -2497,7 +2522,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
@@ -2575,22 +2600,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2898,26 +2923,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -3387,39 +3412,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="H2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="H3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="H4" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="H5" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="H6" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="H7" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="H8" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="H9" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
-    <hyperlink ref="H10" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
-    <hyperlink ref="H11" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
-    <hyperlink ref="H12" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
-    <hyperlink ref="H13" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="H14" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="H16" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="H17" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="H18" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="H19" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.futurlec.com/4000Series/CD4072pr.shtml"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.futurlec.com/4000Series/CD4073pr.shtml"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.futurlec.com/4000Series/CD4075pr.shtml"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.futurlec.com/4000Series/CD4077pr.shtml"/>
+    <hyperlink ref="A16" r:id="rId5" display="https://www.futurlec.com/4000Series/CD4078pr.shtml"/>
+    <hyperlink ref="A17" r:id="rId6" display="https://www.futurlec.com/4000Series/CD4081pr.shtml"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://www.futurlec.com/4000Series/CD4082pr.shtml"/>
+    <hyperlink ref="A19" r:id="rId8" display="https://www.futurlec.com/4000Series/CD4086pr.shtml"/>
+    <hyperlink ref="H2" r:id="rId9"/>
+    <hyperlink ref="H3" r:id="rId10"/>
+    <hyperlink ref="H4" r:id="rId11"/>
+    <hyperlink ref="H5" r:id="rId12"/>
+    <hyperlink ref="H6" r:id="rId13"/>
+    <hyperlink ref="H7" r:id="rId14"/>
+    <hyperlink ref="H8" r:id="rId15"/>
+    <hyperlink ref="H9" r:id="rId16"/>
+    <hyperlink ref="H10" r:id="rId17"/>
+    <hyperlink ref="H11" r:id="rId18"/>
+    <hyperlink ref="H12" r:id="rId19"/>
+    <hyperlink ref="H13" r:id="rId20"/>
+    <hyperlink ref="H14" r:id="rId21"/>
+    <hyperlink ref="H15" r:id="rId22"/>
+    <hyperlink ref="H16" r:id="rId23"/>
+    <hyperlink ref="H17" r:id="rId24"/>
+    <hyperlink ref="H18" r:id="rId25"/>
+    <hyperlink ref="H19" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3580,19 +3605,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3810,22 +3835,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3978,18 +4003,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4207,15 +4232,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G7" r:id="rId6"/>
+    <hyperlink ref="G8" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
file updates for current PELib version
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="2"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="329">
   <si>
     <t>74AC00</t>
   </si>
@@ -1184,12 +1184,33 @@
       <t xml:space="preserve"> (@ TA = +25°C) max</t>
     </r>
   </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/sn74hc153.pdf</t>
+  </si>
+  <si>
+    <t>4:1 mux</t>
+  </si>
+  <si>
+    <t>SN74HC153</t>
+  </si>
+  <si>
+    <t>SN74HC163</t>
+  </si>
+  <si>
+    <t>74xx163 type counter</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/sn74hc163.pdf</t>
+  </si>
+  <si>
+    <t>60pf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1219,6 +1240,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1241,10 +1269,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1560,10 +1589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,6 +1882,16 @@
         <v>319</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
@@ -1867,16 +1906,16 @@
     <hyperlink ref="H11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,6 +2027,16 @@
         <v>275</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -2002,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,6 +2322,16 @@
       </c>
       <c r="H10" s="1" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2293,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,7 +2365,7 @@
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
@@ -2596,6 +2655,58 @@
       </c>
       <c r="I10" s="1" t="s">
         <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>296</v>
+      </c>
+      <c r="F11" t="s">
+        <v>295</v>
+      </c>
+      <c r="G11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G12" t="s">
+        <v>301</v>
+      </c>
+      <c r="H12" t="s">
+        <v>328</v>
+      </c>
+      <c r="I12" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -2616,10 +2727,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2919,6 +3030,16 @@
       </c>
       <c r="I10" s="1" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2943,7 +3064,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,10 +3566,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3601,7 +3722,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>324</v>
+      </c>
       <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>325</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3618,10 +3747,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,6 +3960,16 @@
       </c>
       <c r="G10" s="1" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3851,10 +3990,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,6 +4140,16 @@
         <v>287</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -4015,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4228,6 +4377,16 @@
       </c>
       <c r="G10" s="1" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed table area.xlsx but require minor changes in the future Signed-off-by: Iulia Chereja <chereja_iulia@yahoo.com>
</commit_message>
<xml_diff>
--- a/src/PELib/power_consumption_coefficients.xlsx
+++ b/src/PELib/power_consumption_coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Botix\Desktop\TDC\TDC\src\PELib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iulia\Desktop\repository\src\PELib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD55880A-E5ED-4FFC-8BD7-25D8AB29A6A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF3ADE5-A810-4DFA-AF80-83B0635DD367}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="671" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="74ac" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="339">
   <si>
     <t>74AC00 Quad 2-input NAND Gate</t>
   </si>
@@ -1128,12 +1128,6 @@
     <t>21pf</t>
   </si>
   <si>
-    <t>45pf</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ds/2/149/74AC244-888494.pdf</t>
-  </si>
-  <si>
     <t>https://www.futurlec.com/74AC/74AC244.shtml</t>
   </si>
   <si>
@@ -1215,9 +1209,6 @@
   </si>
   <si>
     <t>MUX2:1</t>
-  </si>
-  <si>
-    <t>NUM163</t>
   </si>
   <si>
     <t>AND4</t>
@@ -1637,25 +1628,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5703125" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1681,7 +1672,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1707,7 +1698,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -1733,7 +1724,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1759,7 +1750,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1785,22 +1776,62 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>326</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>325</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>333</v>
-      </c>
-      <c r="H9" s="1"/>
+        <v>326</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>327</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1815,10 +1846,10 @@
         <v>283</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1826,7 +1857,7 @@
         <v>328</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1841,18 +1872,18 @@
         <v>283</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>282</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1864,121 +1895,38 @@
         <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>309</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>80</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>330</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>283</v>
-      </c>
-      <c r="G13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>341</v>
-      </c>
-      <c r="B14" t="s">
-        <v>282</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
-        <v>284</v>
-      </c>
-      <c r="G14" t="s">
-        <v>309</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>312</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>282</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>288</v>
-      </c>
-      <c r="E15" t="s">
-        <v>287</v>
-      </c>
-      <c r="F15" t="s">
-        <v>281</v>
-      </c>
-      <c r="G15" t="s">
-        <v>310</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>332</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>317</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="H5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="H6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="H7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="H15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2101,12 +2049,12 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD8FE86-977C-4795-BAEF-4C4A14B4FC37}">
   <dimension ref="C8:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -2133,10 +2081,10 @@
   <sheetData>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -2144,10 +2092,10 @@
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G9" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H9">
         <v>5</v>
@@ -2155,10 +2103,10 @@
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2166,10 +2114,10 @@
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G11" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H11">
         <v>6</v>
@@ -2177,10 +2125,10 @@
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H12">
         <v>6</v>
@@ -2188,10 +2136,10 @@
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H13">
         <v>23</v>
@@ -2199,10 +2147,10 @@
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H14">
         <v>4</v>
@@ -2210,10 +2158,10 @@
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -2221,10 +2169,10 @@
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H16">
         <v>7</v>
@@ -2232,10 +2180,10 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G17" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H17">
         <v>8</v>
@@ -2243,37 +2191,37 @@
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2296,9 +2244,10 @@
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="6" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2560,14 +2509,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>316</v>
-      </c>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>317</v>
-      </c>
+      <c r="A12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2590,17 +2535,17 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
@@ -2613,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E1" t="s">
         <v>60</v>
@@ -2894,10 +2839,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -2915,15 +2860,15 @@
         <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -2938,10 +2883,10 @@
         <v>293</v>
       </c>
       <c r="H12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2965,17 +2910,17 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
@@ -3268,14 +3213,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>316</v>
-      </c>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>317</v>
-      </c>
+      <c r="A12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3298,16 +3239,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="6" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3958,13 +3900,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4199,12 +4141,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4377,12 +4319,12 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4616,12 +4558,12 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>